<commit_message>
Avance de PPT de presentación Avance
</commit_message>
<xml_diff>
--- a/PrimerAvance/requirements-analysis.xlsx
+++ b/PrimerAvance/requirements-analysis.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AUTONOMA\Documents\APFP\PrimerAvance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABEL\Downloads\APFP\PrimerAvance\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -205,9 +205,6 @@
     <t>Funcional</t>
   </si>
   <si>
-    <t>Funcioines dministrativas Generenciales</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -263,9 +260,6 @@
   </si>
   <si>
     <t>Técnica</t>
-  </si>
-  <si>
-    <t>Funcion comercial (  asegura la rapida interaccion de los trabajadores con el sistema )</t>
   </si>
   <si>
     <t>La GUI ( interfaz Grafica de usuario ) debe ser accesible y sensilla para todos los usuarios trabajadores.</t>
@@ -351,11 +345,17 @@
   <si>
     <t>El suario Administrador debe poder generar un reporte de las recargas realizadas por su usuario en su jornada</t>
   </si>
+  <si>
+    <t>Funciones dministrativas Gerenciales</t>
+  </si>
+  <si>
+    <t>Funcion comercial (  asegura la rápida interacción de los trabajadores con el sistema )</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -557,24 +557,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -597,14 +597,14 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -886,28 +886,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="71.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="80.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
     <col min="5" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="15"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1001,11 +1001,19 @@
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+    <row r="4" spans="1:26" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1029,18 +1037,18 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" spans="1:26" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="29" t="s">
+    <row r="5" spans="1:26" ht="75" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="29" t="s">
-        <v>28</v>
+      <c r="B5" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1065,18 +1073,18 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:26" ht="135" x14ac:dyDescent="0.2">
-      <c r="A6" s="28" t="s">
-        <v>38</v>
+    <row r="6" spans="1:26" ht="45.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>35</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="29" t="s">
-        <v>30</v>
+      <c r="D6" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1101,18 +1109,18 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" spans="1:26" ht="105" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
+    <row r="7" spans="1:26" ht="30.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="29" t="s">
-        <v>28</v>
+      <c r="D7" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1137,18 +1145,18 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:26" ht="45.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="29" t="s">
+    <row r="8" spans="1:26" ht="90" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="B8" s="11" t="s">
         <v>45</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1173,18 +1181,18 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:26" ht="90" x14ac:dyDescent="0.2">
-      <c r="A9" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="29" t="s">
+    <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="B9" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="29" t="s">
-        <v>30</v>
+      <c r="C9" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1209,19 +1217,11 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="30" x14ac:dyDescent="0.2">
-      <c r="A10" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>45</v>
-      </c>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -1414,10 +1414,10 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1497,7 +1497,7 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -28936,34 +28936,6 @@
       <c r="X999" s="1"/>
       <c r="Y999" s="1"/>
       <c r="Z999" s="1"/>
-    </row>
-    <row r="1000" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1000" s="1"/>
-      <c r="B1000" s="1"/>
-      <c r="C1000" s="1"/>
-      <c r="D1000" s="1"/>
-      <c r="E1000" s="1"/>
-      <c r="F1000" s="1"/>
-      <c r="G1000" s="1"/>
-      <c r="H1000" s="1"/>
-      <c r="I1000" s="1"/>
-      <c r="J1000" s="1"/>
-      <c r="K1000" s="1"/>
-      <c r="L1000" s="1"/>
-      <c r="M1000" s="1"/>
-      <c r="N1000" s="1"/>
-      <c r="O1000" s="1"/>
-      <c r="P1000" s="1"/>
-      <c r="Q1000" s="1"/>
-      <c r="R1000" s="1"/>
-      <c r="S1000" s="1"/>
-      <c r="T1000" s="1"/>
-      <c r="U1000" s="1"/>
-      <c r="V1000" s="1"/>
-      <c r="W1000" s="1"/>
-      <c r="X1000" s="1"/>
-      <c r="Y1000" s="1"/>
-      <c r="Z1000" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -28994,11 +28966,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="15"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -29194,9 +29166,9 @@
       <c r="Z6" s="7"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -29258,7 +29230,7 @@
       <c r="B9" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -29290,7 +29262,7 @@
       <c r="B10" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="16"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -29344,11 +29316,11 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -29377,10 +29349,10 @@
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -29441,10 +29413,10 @@
       <c r="A15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="16"/>
+      <c r="C15" s="17"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -29473,10 +29445,10 @@
       <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="16"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -29503,8 +29475,8 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="18"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -29531,10 +29503,10 @@
     </row>
     <row r="18" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="16"/>
+      <c r="C18" s="17"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -57057,6 +57029,9 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="A17:C17"/>
@@ -57067,9 +57042,6 @@
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B15:C15"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>

</xml_diff>